<commit_message>
feat: plotted cluster vis, and samples from each plotted cluster
</commit_message>
<xml_diff>
--- a/given_files/Parsed_Data.xlsx
+++ b/given_files/Parsed_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Unique H2 Requirements"/>
@@ -5147,7 +5147,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -5518,7 +5518,7 @@
   </sheetPr>
   <dimension ref="A1:E442"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13055,7 +13055,7 @@
   </sheetPr>
   <dimension ref="A1:E555"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13066,7 +13066,7 @@
     <col min="5" max="5" style="6" width="255.57642857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>398</v>
       </c>
@@ -13083,7 +13083,7 @@
         <v>399</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>2001</v>
       </c>
@@ -13100,7 +13100,7 @@
         <v>400</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>2001</v>
       </c>
@@ -13117,7 +13117,7 @@
         <v>401</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>2001</v>
       </c>
@@ -13134,7 +13134,7 @@
         <v>402</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>2001</v>
       </c>
@@ -13151,7 +13151,7 @@
         <v>403</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>2001</v>
       </c>
@@ -13168,7 +13168,7 @@
         <v>404</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
         <v>2001</v>
       </c>
@@ -13185,7 +13185,7 @@
         <v>405</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3">
         <v>2001</v>
       </c>
@@ -13202,7 +13202,7 @@
         <v>406</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3">
         <v>2001</v>
       </c>
@@ -13219,7 +13219,7 @@
         <v>407</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3">
         <v>2001</v>
       </c>
@@ -13236,7 +13236,7 @@
         <v>408</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3">
         <v>2001</v>
       </c>
@@ -13253,7 +13253,7 @@
         <v>409</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3">
         <v>2001</v>
       </c>
@@ -13270,7 +13270,7 @@
         <v>410</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3">
         <v>2001</v>
       </c>
@@ -13287,7 +13287,7 @@
         <v>411</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3">
         <v>2001</v>
       </c>
@@ -13304,7 +13304,7 @@
         <v>412</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3">
         <v>2001</v>
       </c>
@@ -13321,7 +13321,7 @@
         <v>413</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3">
         <v>2001</v>
       </c>
@@ -13338,7 +13338,7 @@
         <v>414</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3">
         <v>2001</v>
       </c>
@@ -13355,7 +13355,7 @@
         <v>415</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3">
         <v>2001</v>
       </c>
@@ -13372,7 +13372,7 @@
         <v>416</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3">
         <v>2001</v>
       </c>
@@ -13389,7 +13389,7 @@
         <v>417</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3">
         <v>2001</v>
       </c>
@@ -13406,7 +13406,7 @@
         <v>418</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3">
         <v>2001</v>
       </c>
@@ -13423,7 +13423,7 @@
         <v>419</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3">
         <v>2001</v>
       </c>
@@ -13440,7 +13440,7 @@
         <v>420</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3">
         <v>2001</v>
       </c>
@@ -13457,7 +13457,7 @@
         <v>421</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3">
         <v>2001</v>
       </c>
@@ -13474,7 +13474,7 @@
         <v>422</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3">
         <v>2001</v>
       </c>
@@ -13491,7 +13491,7 @@
         <v>409</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3">
         <v>2001</v>
       </c>
@@ -13508,7 +13508,7 @@
         <v>423</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="3">
         <v>2001</v>
       </c>
@@ -13525,7 +13525,7 @@
         <v>424</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="3">
         <v>2001</v>
       </c>
@@ -13542,7 +13542,7 @@
         <v>425</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="3">
         <v>2001</v>
       </c>
@@ -13559,7 +13559,7 @@
         <v>426</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="3">
         <v>2001</v>
       </c>
@@ -13576,7 +13576,7 @@
         <v>409</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="3">
         <v>2001</v>
       </c>
@@ -13593,7 +13593,7 @@
         <v>427</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="3">
         <v>2001</v>
       </c>
@@ -13610,7 +13610,7 @@
         <v>428</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="3">
         <v>2001</v>
       </c>
@@ -13627,7 +13627,7 @@
         <v>429</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="3">
         <v>2001</v>
       </c>
@@ -13644,7 +13644,7 @@
         <v>430</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="3">
         <v>2001</v>
       </c>
@@ -13661,7 +13661,7 @@
         <v>431</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="3">
         <v>2001</v>
       </c>
@@ -13678,7 +13678,7 @@
         <v>432</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="3">
         <v>2001</v>
       </c>
@@ -13695,7 +13695,7 @@
         <v>433</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="3">
         <v>2001</v>
       </c>
@@ -13712,7 +13712,7 @@
         <v>434</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="3">
         <v>2001</v>
       </c>
@@ -13729,7 +13729,7 @@
         <v>435</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="3">
         <v>2001</v>
       </c>
@@ -13746,7 +13746,7 @@
         <v>436</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="3">
         <v>2001</v>
       </c>
@@ -13763,7 +13763,7 @@
         <v>437</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="3">
         <v>2001</v>
       </c>
@@ -13780,7 +13780,7 @@
         <v>438</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="3">
         <v>2001</v>
       </c>
@@ -13797,7 +13797,7 @@
         <v>439</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="3">
         <v>2001</v>
       </c>
@@ -13814,7 +13814,7 @@
         <v>440</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="3">
         <v>2001</v>
       </c>
@@ -13831,7 +13831,7 @@
         <v>441</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="3">
         <v>2001</v>
       </c>
@@ -13848,7 +13848,7 @@
         <v>442</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="3">
         <v>2001</v>
       </c>
@@ -13865,7 +13865,7 @@
         <v>443</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="3">
         <v>2001</v>
       </c>
@@ -13882,7 +13882,7 @@
         <v>444</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="3">
         <v>2001</v>
       </c>
@@ -13899,7 +13899,7 @@
         <v>445</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="3">
         <v>2001</v>
       </c>
@@ -13916,7 +13916,7 @@
         <v>446</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="3">
         <v>2001</v>
       </c>
@@ -13933,7 +13933,7 @@
         <v>447</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="3">
         <v>2001</v>
       </c>
@@ -13950,7 +13950,7 @@
         <v>448</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="3">
         <v>2001</v>
       </c>

</xml_diff>